<commit_message>
updated variables on participant-level page
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/AggregateResults/DRE_Variables.xlsx
+++ b/dashboard-ui/src/components/AggregateResults/DRE_Variables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28317"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caci-my.sharepoint.us/personal/jennifer_mcvay_caci_com/Documents/ITM-FAITH-MD/Experimental Design/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{782E65E4-D5E8-46AE-87CD-531AED5EAE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4150447-CF65-4209-8A67-FD8B2289F283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="945" yWindow="720" windowWidth="27855" windowHeight="15480" xr2:uid="{0CF369EF-FF88-492D-A804-82D5E90C57ED}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="84">
   <si>
     <t>Variable Group</t>
   </si>
@@ -240,34 +240,46 @@
     <t>The ST Value of Life scenario the participant completed in the VR simulation</t>
   </si>
   <si>
+    <t>QOL_KDE_Text</t>
+  </si>
+  <si>
+    <t>KDMA measurement from text probe responses for the ST Quality of Life scenario</t>
+  </si>
+  <si>
+    <t>Hyperlink to Graph</t>
+  </si>
+  <si>
+    <t>From TA1 Server</t>
+  </si>
+  <si>
     <t>QOL_KDMA_Text</t>
   </si>
   <si>
-    <t>KDMA measurement from text probe responses for the ST Quality of Life scenario</t>
-  </si>
-  <si>
-    <t>Hyperlink to Graph</t>
-  </si>
-  <si>
-    <t>From TA1 Server</t>
+    <t>QOL_KDE_Sim</t>
+  </si>
+  <si>
+    <t>KDMA measurement from sim probe responses for the ST Quality of Life Scenario</t>
   </si>
   <si>
     <t>QOL_KDMA_Sim</t>
   </si>
   <si>
-    <t>KDMA measurement from sim probe responses for the ST Quality of Life Scenario</t>
+    <t>VOL_KDE_Text</t>
+  </si>
+  <si>
+    <t>KDMA measurement from text probe responses for the ST Value of Life scenario</t>
   </si>
   <si>
     <t>VOL_KDMA_Text</t>
   </si>
   <si>
-    <t>KDMA measurement from text probe responses for the ST Value of Life scenario</t>
+    <t>VOL_KDE_Sim</t>
+  </si>
+  <si>
+    <t>KDMA measurement from sim probe responses for the ST Value of Life Scenario</t>
   </si>
   <si>
     <t>VOL_KDMA_Sim</t>
-  </si>
-  <si>
-    <t>KDMA measurement from sim probe responses for the ST Value of Life Scenario</t>
   </si>
   <si>
     <t>MJ_KDMA_Text</t>
@@ -789,10 +801,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B809285-AF47-49CD-A271-20BB7A909323}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1048544" workbookViewId="0">
-      <selection activeCell="A1048576" sqref="A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1152,10 +1164,10 @@
         <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="E19" t="s">
         <v>47</v>
@@ -1169,10 +1181,10 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" t="s">
-        <v>69</v>
       </c>
       <c r="D20" t="s">
         <v>64</v>
@@ -1189,13 +1201,13 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>71</v>
+        <v>69</v>
+      </c>
+      <c r="C21" t="s">
+        <v>68</v>
       </c>
       <c r="D21" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
         <v>47</v>
@@ -1209,13 +1221,13 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E22" t="s">
         <v>47</v>
@@ -1229,10 +1241,10 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
         <v>27</v>
@@ -1249,13 +1261,13 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>76</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
+        <v>73</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="E24" t="s">
         <v>47</v>
@@ -1269,10 +1281,10 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
-      </c>
-      <c r="C25" t="s">
-        <v>79</v>
+        <v>75</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>74</v>
       </c>
       <c r="D25" t="s">
         <v>27</v>
@@ -1281,6 +1293,86 @@
         <v>47</v>
       </c>
       <c r="F25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>47</v>
+      </c>
+      <c r="F26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>47</v>
+      </c>
+      <c r="F27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" t="s">
+        <v>47</v>
+      </c>
+      <c r="F28" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>